<commit_message>
importing Data from Properties file done
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/Providerss.xlsx
+++ b/src/main/resources/testData/Providerss.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\khale\IdeaProjects\Noon_Automation\src\main\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653D8AC8-B349-4F68-B298-317D22F37B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D4548A-94C5-4383-9EBF-A0F5A2FDCD7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>min value</t>
   </si>
   <si>
     <t>max value</t>
+  </si>
+  <si>
+    <t>fgfdg</t>
+  </si>
+  <si>
+    <t>tertret</t>
   </si>
 </sst>
 </file>
@@ -367,7 +373,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,10 +432,20 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>5454545</v>
+      </c>
+      <c r="B8" s="2">
+        <v>321</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>

</xml_diff>